<commit_message>
update JP travel plan
</commit_message>
<xml_diff>
--- a/plan/日本旅行行程安排_v2.xlsx
+++ b/plan/日本旅行行程安排_v2.xlsx
@@ -54,10 +54,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>大阪 - 关西</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1）南海快铁 Rapit 是关西机场前往难波、心斋桥地区的最好选择，35分钟， JPY1390
 2) 普通日铁快车称为关空快速列车 kanku kaisoku，到日铁难波站JPY1030， 56分钟</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -146,6 +142,10 @@
   </si>
   <si>
     <t>逛街买东西</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大阪 - 关西 - 上海</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -505,7 +505,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -530,7 +530,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="67.5">
@@ -538,16 +538,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -555,13 +555,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -570,13 +570,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -585,13 +585,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -603,7 +603,7 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="4"/>
     </row>
@@ -629,10 +629,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="67.5">
@@ -640,13 +640,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -654,10 +654,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="54">
@@ -665,10 +665,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D11" s="1"/>
     </row>

</xml_diff>